<commit_message>
Updated Commit moving files to resources.
</commit_message>
<xml_diff>
--- a/The Harpoon/Comparison Template.xlsx
+++ b/The Harpoon/Comparison Template.xlsx
@@ -9,9 +9,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Fund Management\Fund Management Team Files\FM Personal Folders\Richard\PycharmProjects\The Harpoon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3B75CD3-5AE7-4419-99F2-7CBA7A2D32F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B61DF8-E519-4E02-9C08-10A24827745A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28560" yWindow="360" windowWidth="29040" windowHeight="15840" tabRatio="757" activeTab="2" xr2:uid="{999F52BA-D2FF-425D-8559-FEC8672B03CF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="757" activeTab="7" xr2:uid="{999F52BA-D2FF-425D-8559-FEC8672B03CF}"/>
   </bookViews>
   <sheets>
     <sheet name="Portfolio holdings" sheetId="1" r:id="rId1"/>
@@ -486,9 +486,6 @@
     <t>ytd_performance_margetts</t>
   </si>
   <si>
-    <t>% and the client returning c.</t>
-  </si>
-  <si>
     <t>ytd_performance_client</t>
   </si>
   <si>
@@ -616,6 +613,9 @@
   </si>
   <si>
     <t xml:space="preserve"> exposure to cash and bonds compared to the Margetts RR </t>
+  </si>
+  <si>
+    <t>% and the client's portfolio returning c.</t>
   </si>
 </sst>
 </file>
@@ -3016,7 +3016,7 @@
       </c>
       <c r="B5" s="67">
         <f ca="1">'Portfolio Comparison'!H19</f>
-        <v>45007</v>
+        <v>45035</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3139,7 +3139,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -3162,7 +3162,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -3185,7 +3185,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -3208,12 +3208,12 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B31" s="5">
         <f>'Performance Comparison'!C5</f>
@@ -3227,12 +3227,12 @@
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>
@@ -3295,7 +3295,7 @@
         <v>18</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3399,7 +3399,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -3646,7 +3646,7 @@
       </c>
       <c r="H19" s="59">
         <f ca="1">TODAY()</f>
-        <v>45007</v>
+        <v>45035</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -3776,7 +3776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04798506-4781-40D5-823A-182FA1CD1F43}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -3827,7 +3827,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="83" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B6" s="84"/>
       <c r="C6" s="85"/>
@@ -3869,7 +3869,7 @@
     </row>
     <row r="12" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="56" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B12" s="81"/>
       <c r="C12" s="82"/>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" s="49" t="s">
         <v>76</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="48" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B6" s="49" t="s">
         <v>80</v>
@@ -4624,7 +4624,7 @@
     </row>
     <row r="8" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -4634,7 +4634,7 @@
     </row>
     <row r="10" spans="1:2" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -4707,7 +4707,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="49" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>75</v>
@@ -4829,7 +4829,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="51" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B18" t="s">
         <v>111</v>
@@ -4848,7 +4848,7 @@
         <v>86</v>
       </c>
       <c r="B20" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -4858,7 +4858,7 @@
     </row>
     <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -4998,12 +4998,12 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -5021,7 +5021,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DB1CBFA-E26B-45DE-8EC2-52F7369188ED}">
   <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5079,15 +5081,15 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B7" s="49" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="49" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B8" s="49" t="s">
         <v>121</v>
@@ -5103,10 +5105,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="49" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5119,10 +5121,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -5154,7 +5156,7 @@
         <v>118</v>
       </c>
       <c r="B16" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5170,15 +5172,15 @@
         <v>124</v>
       </c>
       <c r="B18" s="49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="49" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B19" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -5188,7 +5190,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -5218,17 +5220,17 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="49" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -5258,7 +5260,7 @@
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="51" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -5298,17 +5300,17 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="49" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="49" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -5328,12 +5330,12 @@
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="49" t="s">
-        <v>138</v>
+        <v>181</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="49" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
@@ -5358,7 +5360,7 @@
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="49" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -5368,7 +5370,7 @@
     </row>
     <row r="57" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
@@ -5378,17 +5380,17 @@
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="49" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="49" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -5398,7 +5400,7 @@
     </row>
     <row r="63" spans="1:1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="51" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
   </sheetData>
@@ -5423,7 +5425,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="49" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B1" t="s">
         <v>116</v>
@@ -5439,7 +5441,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B3" s="49" t="s">
         <v>75</v>
@@ -5452,7 +5454,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="49" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -5462,7 +5464,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="49" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5472,7 +5474,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -5482,7 +5484,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="49" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -5492,7 +5494,7 @@
     </row>
     <row r="13" spans="1:2" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="49" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -5502,7 +5504,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="49" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -5512,7 +5514,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="51" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -5522,7 +5524,7 @@
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
@@ -5532,7 +5534,7 @@
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="51" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
@@ -5542,7 +5544,7 @@
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="49" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -5552,6 +5554,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="4f0e86fe-6553-4263-90f0-a5f33ec9ea3e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d0fbbff-9b87-4770-aee3-1c1fe6f9d7d6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010006330D3C405A7B458131DD13BEC39F68" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c1f4ab7ee5ee4a6e44ce996f753e5371">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3d0fbbff-9b87-4770-aee3-1c1fe6f9d7d6" xmlns:ns3="4f0e86fe-6553-4263-90f0-a5f33ec9ea3e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="95cfbebb277ee8150f17ba2039e1cb43" ns2:_="" ns3:_="">
     <xsd:import namespace="3d0fbbff-9b87-4770-aee3-1c1fe6f9d7d6"/>
@@ -5768,27 +5790,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25603E06-45B5-4D27-B898-B62DFF416807}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3d0fbbff-9b87-4770-aee3-1c1fe6f9d7d6"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="4f0e86fe-6553-4263-90f0-a5f33ec9ea3e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="4f0e86fe-6553-4263-90f0-a5f33ec9ea3e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3d0fbbff-9b87-4770-aee3-1c1fe6f9d7d6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A30221F-34E3-405C-B685-3B34165B9140}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B48DFE71-66B2-477D-8E6F-9017DCCC4F9B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5805,29 +5832,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9A30221F-34E3-405C-B685-3B34165B9140}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25603E06-45B5-4D27-B898-B62DFF416807}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3d0fbbff-9b87-4770-aee3-1c1fe6f9d7d6"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="4f0e86fe-6553-4263-90f0-a5f33ec9ea3e"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>